<commit_message>
Added five tests for login with different valid usernames
</commit_message>
<xml_diff>
--- a/src/test/java/TestData.xlsx
+++ b/src/test/java/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\IdeaProjects\SwagLabs\src\test\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C58310E-12F6-4607-93E0-EB32EC787F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82BEC50-7B6F-4FF7-B7A3-45DBEA875CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6B670275-6032-46DE-ACD2-F063BC859524}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Valid username</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>sausage*?</t>
+  </si>
+  <si>
+    <t>visual_user</t>
+  </si>
+  <si>
+    <t>visualuser</t>
+  </si>
+  <si>
+    <t>saucelabs</t>
   </si>
 </sst>
 </file>
@@ -445,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE466FA-3E66-4A37-A95D-FAC97F9A3FF4}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,46 +498,57 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added three pages and one test class for checkout
</commit_message>
<xml_diff>
--- a/src/test/java/TestData.xlsx
+++ b/src/test/java/TestData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\IdeaProjects\SwagLabs\src\test\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82BEC50-7B6F-4FF7-B7A3-45DBEA875CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA00C1C-6D48-4078-BFAA-6E7BDB37597A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6B670275-6032-46DE-ACD2-F063BC859524}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{6B670275-6032-46DE-ACD2-F063BC859524}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="CheckoutInfo" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Valid username</t>
   </si>
@@ -94,6 +95,33 @@
   </si>
   <si>
     <t>saucelabs</t>
+  </si>
+  <si>
+    <t>First name</t>
+  </si>
+  <si>
+    <t>Last name</t>
+  </si>
+  <si>
+    <t>Zip/Postal Code</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Parker</t>
+  </si>
+  <si>
+    <t>Tom</t>
+  </si>
+  <si>
+    <t>Davis</t>
+  </si>
+  <si>
+    <t>1223A</t>
+  </si>
+  <si>
+    <t>3455B</t>
   </si>
 </sst>
 </file>
@@ -456,7 +484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE466FA-3E66-4A37-A95D-FAC97F9A3FF4}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -554,4 +582,58 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D6A180C-627D-4C86-8C68-3F7DFEC9561B}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.88671875" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>